<commit_message>
Improve reader service test
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B53F98-95AF-462A-BBA0-64C10683CE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA11A11-EC30-4057-9E4F-F425D35E5206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10880" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Cell A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell B5</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADF6F0E-2A17-4FF0-B419-BBA98FA39085}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +460,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve reader service tests (#37)
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B53F98-95AF-462A-BBA0-64C10683CE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA11A11-EC30-4057-9E4F-F425D35E5206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10880" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Cell A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell A5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell B4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cell B5</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADF6F0E-2A17-4FF0-B419-BBA98FA39085}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +460,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: specify sheets to extract when reading a file
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA11A11-EC30-4057-9E4F-F425D35E5206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF89342-5941-E84E-99CD-FD081E69462B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10880" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="-2340" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -52,16 +53,43 @@
   </si>
   <si>
     <t xml:space="preserve"> Cell B5</t>
+  </si>
+  <si>
+    <t>feuil2 A1</t>
+  </si>
+  <si>
+    <t>feuil2 A2</t>
+  </si>
+  <si>
+    <t>feuil2 A4</t>
+  </si>
+  <si>
+    <t>feuil2 B2</t>
+  </si>
+  <si>
+    <t>feuil2 B3</t>
+  </si>
+  <si>
+    <t>feuil2 B4</t>
+  </si>
+  <si>
+    <t>feuil2 B1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,13 +458,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADF6F0E-2A17-4FF0-B419-BBA98FA39085}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -444,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -452,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -460,12 +488,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -476,4 +504,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7D2E04-97CF-EF45-9E2D-68F425CFBF33}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Specify sheets to extract when reading a file (#43)
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA11A11-EC30-4057-9E4F-F425D35E5206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF89342-5941-E84E-99CD-FD081E69462B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10880" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="-2340" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -52,16 +53,43 @@
   </si>
   <si>
     <t xml:space="preserve"> Cell B5</t>
+  </si>
+  <si>
+    <t>feuil2 A1</t>
+  </si>
+  <si>
+    <t>feuil2 A2</t>
+  </si>
+  <si>
+    <t>feuil2 A4</t>
+  </si>
+  <si>
+    <t>feuil2 B2</t>
+  </si>
+  <si>
+    <t>feuil2 B3</t>
+  </si>
+  <si>
+    <t>feuil2 B4</t>
+  </si>
+  <si>
+    <t>feuil2 B1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,13 +458,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADF6F0E-2A17-4FF0-B419-BBA98FA39085}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -444,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -452,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -460,12 +488,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -476,4 +504,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7D2E04-97CF-EF45-9E2D-68F425CFBF33}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add reader options that can allow user to choose stylesheet and starting coordinates
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF89342-5941-E84E-99CD-FD081E69462B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519AB2EB-2D16-4E44-B663-044F90079044}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-2340" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -70,10 +70,13 @@
     <t>feuil2 B3</t>
   </si>
   <si>
-    <t>feuil2 B4</t>
-  </si>
-  <si>
     <t>feuil2 B1</t>
+  </si>
+  <si>
+    <t>feuil2 B5</t>
+  </si>
+  <si>
+    <t>feuil2 A5</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7D2E04-97CF-EF45-9E2D-68F425CFBF33}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -521,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,8 +544,13 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: allow user to choose stylesheet and starting coordinates (#44)
</commit_message>
<xml_diff>
--- a/test/input.xlsx
+++ b/test/input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF89342-5941-E84E-99CD-FD081E69462B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519AB2EB-2D16-4E44-B663-044F90079044}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-2340" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve"> Cell B2</t>
   </si>
@@ -70,10 +70,13 @@
     <t>feuil2 B3</t>
   </si>
   <si>
-    <t>feuil2 B4</t>
-  </si>
-  <si>
     <t>feuil2 B1</t>
+  </si>
+  <si>
+    <t>feuil2 B5</t>
+  </si>
+  <si>
+    <t>feuil2 A5</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7D2E04-97CF-EF45-9E2D-68F425CFBF33}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -521,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,8 +544,13 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>